<commit_message>
Acrescentado o Neo4jPersister ao pacote lattes_scrapper.py
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -518,13 +518,13 @@
         <v>1465</v>
       </c>
       <c r="I2" t="n">
-        <v>480</v>
+        <v>620</v>
       </c>
       <c r="J2" t="n">
-        <v>11485</v>
+        <v>11625</v>
       </c>
       <c r="K2" t="n">
-        <v>99.15000000000001</v>
+        <v>30.51</v>
       </c>
     </row>
     <row r="3">
@@ -561,7 +561,7 @@
         <v>8855</v>
       </c>
       <c r="K3" t="n">
-        <v>98.45999999999999</v>
+        <v>11.63</v>
       </c>
     </row>
     <row r="4">
@@ -598,7 +598,7 @@
         <v>8695</v>
       </c>
       <c r="K4" t="n">
-        <v>100</v>
+        <v>29.13</v>
       </c>
     </row>
     <row r="5">
@@ -635,7 +635,7 @@
         <v>4490</v>
       </c>
       <c r="K5" t="n">
-        <v>100</v>
+        <v>12.28</v>
       </c>
     </row>
     <row r="6">
@@ -672,7 +672,7 @@
         <v>4175</v>
       </c>
       <c r="K6" t="n">
-        <v>95.18000000000001</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="7">
@@ -709,7 +709,7 @@
         <v>3755</v>
       </c>
       <c r="K7" t="n">
-        <v>98.78</v>
+        <v>57.14</v>
       </c>
     </row>
     <row r="8">
@@ -746,7 +746,7 @@
         <v>3660</v>
       </c>
       <c r="K8" t="n">
-        <v>98.81</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +783,7 @@
         <v>3640</v>
       </c>
       <c r="K9" t="n">
-        <v>98.34</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="10">
@@ -814,13 +814,13 @@
         <v>220</v>
       </c>
       <c r="I10" t="n">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="J10" t="n">
-        <v>3530</v>
+        <v>3620</v>
       </c>
       <c r="K10" t="n">
-        <v>95.5</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="11">
@@ -857,7 +857,7 @@
         <v>3380</v>
       </c>
       <c r="K11" t="n">
-        <v>100</v>
+        <v>15.56</v>
       </c>
     </row>
     <row r="12">
@@ -894,7 +894,7 @@
         <v>3180</v>
       </c>
       <c r="K12" t="n">
-        <v>95.56</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="13">
@@ -931,7 +931,7 @@
         <v>3085</v>
       </c>
       <c r="K13" t="n">
-        <v>100</v>
+        <v>27.45</v>
       </c>
     </row>
     <row r="14">
@@ -968,7 +968,7 @@
         <v>2765</v>
       </c>
       <c r="K14" t="n">
-        <v>65.56999999999999</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="15">
@@ -1005,7 +1005,7 @@
         <v>2745</v>
       </c>
       <c r="K15" t="n">
-        <v>94.39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -1042,7 +1042,7 @@
         <v>2730</v>
       </c>
       <c r="K16" t="n">
-        <v>100</v>
+        <v>14.71</v>
       </c>
     </row>
     <row r="17">
@@ -1079,7 +1079,7 @@
         <v>2715</v>
       </c>
       <c r="K17" t="n">
-        <v>94.87</v>
+        <v>34.88</v>
       </c>
     </row>
     <row r="18">
@@ -1116,7 +1116,7 @@
         <v>2525</v>
       </c>
       <c r="K18" t="n">
-        <v>100</v>
+        <v>36.84</v>
       </c>
     </row>
     <row r="19">
@@ -1153,7 +1153,7 @@
         <v>2415</v>
       </c>
       <c r="K19" t="n">
-        <v>100</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="20">
@@ -1190,7 +1190,7 @@
         <v>2270</v>
       </c>
       <c r="K20" t="n">
-        <v>98.77</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="21">
@@ -1227,7 +1227,7 @@
         <v>2260</v>
       </c>
       <c r="K21" t="n">
-        <v>100</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="22">
@@ -1264,7 +1264,7 @@
         <v>2145</v>
       </c>
       <c r="K22" t="n">
-        <v>98.11</v>
+        <v>30.56</v>
       </c>
     </row>
     <row r="23">
@@ -1301,7 +1301,7 @@
         <v>2125</v>
       </c>
       <c r="K23" t="n">
-        <v>97.56</v>
+        <v>23.53</v>
       </c>
     </row>
     <row r="24">
@@ -1338,7 +1338,7 @@
         <v>2105</v>
       </c>
       <c r="K24" t="n">
-        <v>95.23999999999999</v>
+        <v>65.62</v>
       </c>
     </row>
     <row r="25">
@@ -1375,7 +1375,7 @@
         <v>2105</v>
       </c>
       <c r="K25" t="n">
-        <v>83.64</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="26">
@@ -1412,7 +1412,7 @@
         <v>2100</v>
       </c>
       <c r="K26" t="n">
-        <v>97.92</v>
+        <v>19.35</v>
       </c>
     </row>
     <row r="27">
@@ -1449,7 +1449,7 @@
         <v>2090</v>
       </c>
       <c r="K27" t="n">
-        <v>100</v>
+        <v>65.38</v>
       </c>
     </row>
     <row r="28">
@@ -1486,7 +1486,7 @@
         <v>2090</v>
       </c>
       <c r="K28" t="n">
-        <v>100</v>
+        <v>58.82</v>
       </c>
     </row>
     <row r="29">
@@ -1523,7 +1523,7 @@
         <v>1955</v>
       </c>
       <c r="K29" t="n">
-        <v>98.39</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="30">
@@ -1560,7 +1560,7 @@
         <v>1880</v>
       </c>
       <c r="K30" t="n">
-        <v>100</v>
+        <v>72.73</v>
       </c>
     </row>
     <row r="31">
@@ -1597,7 +1597,7 @@
         <v>1850</v>
       </c>
       <c r="K31" t="n">
-        <v>88.89</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="32">
@@ -1634,7 +1634,7 @@
         <v>1730</v>
       </c>
       <c r="K32" t="n">
-        <v>99.58</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="33">
@@ -1671,7 +1671,7 @@
         <v>1710</v>
       </c>
       <c r="K33" t="n">
-        <v>97.44</v>
+        <v>26.09</v>
       </c>
     </row>
     <row r="34">
@@ -1708,7 +1708,7 @@
         <v>1685</v>
       </c>
       <c r="K34" t="n">
-        <v>91.36</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="35">
@@ -1745,7 +1745,7 @@
         <v>1630</v>
       </c>
       <c r="K35" t="n">
-        <v>74.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1782,7 +1782,7 @@
         <v>1630</v>
       </c>
       <c r="K36" t="n">
-        <v>100</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="37">
@@ -1819,7 +1819,7 @@
         <v>1590</v>
       </c>
       <c r="K37" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1856,7 +1856,7 @@
         <v>1560</v>
       </c>
       <c r="K38" t="n">
-        <v>100</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="39">
@@ -1893,7 +1893,7 @@
         <v>1450</v>
       </c>
       <c r="K39" t="n">
-        <v>89.47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40">
@@ -1930,7 +1930,7 @@
         <v>1415</v>
       </c>
       <c r="K40" t="n">
-        <v>89.13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41">
@@ -1967,7 +1967,7 @@
         <v>1405</v>
       </c>
       <c r="K41" t="n">
-        <v>100</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="42">
@@ -2004,7 +2004,7 @@
         <v>1390</v>
       </c>
       <c r="K42" t="n">
-        <v>100</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="43">
@@ -2041,7 +2041,7 @@
         <v>1305</v>
       </c>
       <c r="K43" t="n">
-        <v>99.34999999999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
@@ -2078,7 +2078,7 @@
         <v>1195</v>
       </c>
       <c r="K44" t="n">
-        <v>100</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="45">
@@ -2115,7 +2115,7 @@
         <v>1185</v>
       </c>
       <c r="K45" t="n">
-        <v>98.94</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="46">
@@ -2152,7 +2152,7 @@
         <v>965</v>
       </c>
       <c r="K46" t="n">
-        <v>88.23999999999999</v>
+        <v>26.67</v>
       </c>
     </row>
     <row r="47">
@@ -2189,7 +2189,7 @@
         <v>900</v>
       </c>
       <c r="K47" t="n">
-        <v>100</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="48">
@@ -2226,7 +2226,7 @@
         <v>895</v>
       </c>
       <c r="K48" t="n">
-        <v>100</v>
+        <v>52.94</v>
       </c>
     </row>
     <row r="49">
@@ -2263,7 +2263,7 @@
         <v>875</v>
       </c>
       <c r="K49" t="n">
-        <v>94.12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50">
@@ -2300,7 +2300,7 @@
         <v>810</v>
       </c>
       <c r="K50" t="n">
-        <v>78.26000000000001</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -2337,7 +2337,7 @@
         <v>800</v>
       </c>
       <c r="K51" t="n">
-        <v>100</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="52">
@@ -2374,7 +2374,7 @@
         <v>790</v>
       </c>
       <c r="K52" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53">
@@ -2411,7 +2411,7 @@
         <v>790</v>
       </c>
       <c r="K53" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54">
@@ -2448,7 +2448,7 @@
         <v>730</v>
       </c>
       <c r="K54" t="n">
-        <v>100</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="55">
@@ -2485,7 +2485,7 @@
         <v>540</v>
       </c>
       <c r="K55" t="n">
-        <v>65.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2522,7 +2522,7 @@
         <v>495</v>
       </c>
       <c r="K56" t="n">
-        <v>96.15000000000001</v>
+        <v>23.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrigido tratamento de homônimos funcionando até 20 resultados, ainda falha para mais que isso.
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,13 +555,13 @@
         <v>1610</v>
       </c>
       <c r="I3" t="n">
-        <v>435</v>
+        <v>805</v>
       </c>
       <c r="J3" t="n">
-        <v>8855</v>
+        <v>9225</v>
       </c>
       <c r="K3" t="n">
-        <v>11.63</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="4">
@@ -703,124 +703,124 @@
         <v>290</v>
       </c>
       <c r="I7" t="n">
-        <v>380</v>
+        <v>470</v>
       </c>
       <c r="J7" t="n">
-        <v>3755</v>
+        <v>3845</v>
       </c>
       <c r="K7" t="n">
-        <v>57.14</v>
+        <v>57.89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Lis Ribeiro do Valle Antonelli</t>
+          <t>Rodrigo Pedro Pinto Soares</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>310</v>
+        <v>540</v>
       </c>
       <c r="C8" t="n">
-        <v>630</v>
+        <v>560</v>
       </c>
       <c r="D8" t="n">
-        <v>690</v>
+        <v>620</v>
       </c>
       <c r="E8" t="n">
-        <v>470</v>
+        <v>520</v>
       </c>
       <c r="F8" t="n">
-        <v>670</v>
+        <v>750</v>
       </c>
       <c r="G8" t="n">
-        <v>530</v>
+        <v>150</v>
       </c>
       <c r="H8" t="n">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="I8" t="n">
-        <v>90</v>
+        <v>350</v>
       </c>
       <c r="J8" t="n">
-        <v>3660</v>
+        <v>3710</v>
       </c>
       <c r="K8" t="n">
-        <v>14.89</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Correa de Oliveira</t>
+          <t>Lis Ribeiro do Valle Antonelli</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1290</v>
+        <v>310</v>
       </c>
       <c r="C9" t="n">
-        <v>360</v>
+        <v>630</v>
       </c>
       <c r="D9" t="n">
-        <v>770</v>
+        <v>690</v>
       </c>
       <c r="E9" t="n">
-        <v>360</v>
+        <v>470</v>
       </c>
       <c r="F9" t="n">
-        <v>360</v>
+        <v>670</v>
       </c>
       <c r="G9" t="n">
-        <v>230</v>
+        <v>530</v>
       </c>
       <c r="H9" t="n">
         <v>270</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J9" t="n">
-        <v>3640</v>
+        <v>3660</v>
       </c>
       <c r="K9" t="n">
-        <v>8.33</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Pedro Pinto Soares</t>
+          <t>Rodrigo Correa de Oliveira</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>540</v>
+        <v>1290</v>
       </c>
       <c r="C10" t="n">
-        <v>560</v>
+        <v>360</v>
       </c>
       <c r="D10" t="n">
-        <v>620</v>
+        <v>770</v>
       </c>
       <c r="E10" t="n">
-        <v>520</v>
+        <v>360</v>
       </c>
       <c r="F10" t="n">
-        <v>750</v>
+        <v>360</v>
       </c>
       <c r="G10" t="n">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="H10" t="n">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="I10" t="n">
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>3620</v>
+        <v>3640</v>
       </c>
       <c r="K10" t="n">
-        <v>10.53</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="11">
@@ -937,75 +937,75 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Antonio Mauro Rezende</t>
+          <t>Celia Maria Ferreira Gontijo</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>230</v>
+        <v>480</v>
       </c>
       <c r="C14" t="n">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="D14" t="n">
-        <v>480</v>
+        <v>390</v>
       </c>
       <c r="E14" t="n">
-        <v>560</v>
+        <v>500</v>
       </c>
       <c r="F14" t="n">
-        <v>450</v>
+        <v>260</v>
       </c>
       <c r="G14" t="n">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="H14" t="n">
-        <v>390</v>
+        <v>260</v>
       </c>
       <c r="I14" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="J14" t="n">
-        <v>2765</v>
+        <v>2785</v>
       </c>
       <c r="K14" t="n">
-        <v>7.14</v>
+        <v>19.51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Celia Maria Ferreira Gontijo</t>
+          <t>Antonio Mauro Rezende</t>
         </is>
       </c>
       <c r="B15" t="n">
+        <v>230</v>
+      </c>
+      <c r="C15" t="n">
+        <v>360</v>
+      </c>
+      <c r="D15" t="n">
         <v>480</v>
       </c>
-      <c r="C15" t="n">
-        <v>585</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>560</v>
+      </c>
+      <c r="F15" t="n">
+        <v>450</v>
+      </c>
+      <c r="G15" t="n">
+        <v>280</v>
+      </c>
+      <c r="H15" t="n">
         <v>390</v>
       </c>
-      <c r="E15" t="n">
-        <v>500</v>
-      </c>
-      <c r="F15" t="n">
-        <v>260</v>
-      </c>
-      <c r="G15" t="n">
-        <v>270</v>
-      </c>
-      <c r="H15" t="n">
-        <v>260</v>
-      </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J15" t="n">
-        <v>2745</v>
+        <v>2765</v>
       </c>
       <c r="K15" t="n">
-        <v>20</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="16">
@@ -1159,581 +1159,581 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Cristiana Ferreira Alves de Brito</t>
+          <t>Márcio Sobreira Silva Araújo</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>370</v>
+        <v>145</v>
       </c>
       <c r="C20" t="n">
-        <v>440</v>
+        <v>665</v>
       </c>
       <c r="D20" t="n">
-        <v>530</v>
+        <v>180</v>
       </c>
       <c r="E20" t="n">
-        <v>270</v>
+        <v>215</v>
       </c>
       <c r="F20" t="n">
-        <v>330</v>
+        <v>185</v>
       </c>
       <c r="G20" t="n">
-        <v>160</v>
+        <v>475</v>
       </c>
       <c r="H20" t="n">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="J20" t="n">
-        <v>2270</v>
+        <v>2285</v>
       </c>
       <c r="K20" t="n">
-        <v>43.75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Alessandra Aparecida Guarneri</t>
+          <t>Cristiana Ferreira Alves de Brito</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C21" t="n">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="D21" t="n">
-        <v>210</v>
+        <v>530</v>
       </c>
       <c r="E21" t="n">
-        <v>430</v>
+        <v>270</v>
       </c>
       <c r="F21" t="n">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="G21" t="n">
-        <v>260</v>
+        <v>160</v>
       </c>
       <c r="H21" t="n">
-        <v>360</v>
+        <v>170</v>
       </c>
       <c r="I21" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>2260</v>
+        <v>2270</v>
       </c>
       <c r="K21" t="n">
-        <v>22.22</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Antonio Pascoal Xavier</t>
+          <t>Alessandra Aparecida Guarneri</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="C22" t="n">
-        <v>545</v>
+        <v>220</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="E22" t="n">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F22" t="n">
-        <v>370</v>
+        <v>340</v>
       </c>
       <c r="G22" t="n">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="H22" t="n">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="I22" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="J22" t="n">
-        <v>2145</v>
+        <v>2260</v>
       </c>
       <c r="K22" t="n">
-        <v>30.56</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Márcio Sobreira Silva Araújo</t>
+          <t>Marcelo Antonio Pascoal Xavier</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="C23" t="n">
-        <v>665</v>
+        <v>545</v>
       </c>
       <c r="D23" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>215</v>
+        <v>435</v>
       </c>
       <c r="F23" t="n">
-        <v>185</v>
+        <v>370</v>
       </c>
       <c r="G23" t="n">
-        <v>475</v>
+        <v>200</v>
       </c>
       <c r="H23" t="n">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="I23" t="n">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="J23" t="n">
-        <v>2125</v>
+        <v>2145</v>
       </c>
       <c r="K23" t="n">
-        <v>23.53</v>
+        <v>30.56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Rubens Lima do Monte Neto</t>
+          <t>Taís Nóbrega de Sousa</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="C24" t="n">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="D24" t="n">
-        <v>40</v>
+        <v>310</v>
       </c>
       <c r="E24" t="n">
-        <v>280</v>
+        <v>350</v>
       </c>
       <c r="F24" t="n">
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="G24" t="n">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="H24" t="n">
-        <v>330</v>
+        <v>160</v>
       </c>
       <c r="I24" t="n">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="J24" t="n">
-        <v>2105</v>
+        <v>2130</v>
       </c>
       <c r="K24" t="n">
-        <v>17.65</v>
+        <v>62.96</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Marina de Moraes Mourão</t>
+          <t>Rubens Lima do Monte Neto</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>460</v>
+        <v>80</v>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>400</v>
       </c>
       <c r="D25" t="n">
-        <v>390</v>
+        <v>40</v>
       </c>
       <c r="E25" t="n">
+        <v>280</v>
+      </c>
+      <c r="F25" t="n">
+        <v>420</v>
+      </c>
+      <c r="G25" t="n">
+        <v>425</v>
+      </c>
+      <c r="H25" t="n">
         <v>330</v>
       </c>
-      <c r="F25" t="n">
-        <v>220</v>
-      </c>
-      <c r="G25" t="n">
-        <v>410</v>
-      </c>
-      <c r="H25" t="n">
-        <v>200</v>
-      </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="J25" t="n">
-        <v>2100</v>
+        <v>2105</v>
       </c>
       <c r="K25" t="n">
-        <v>19.35</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Ana Lúcia Teles Rabello</t>
+          <t>Pedro Augusto Alves</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>610</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="D26" t="n">
-        <v>610</v>
+        <v>250</v>
       </c>
       <c r="E26" t="n">
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="F26" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="G26" t="n">
-        <v>180</v>
+        <v>460</v>
       </c>
       <c r="H26" t="n">
-        <v>20</v>
+        <v>380</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="J26" t="n">
-        <v>2090</v>
+        <v>2105</v>
       </c>
       <c r="K26" t="n">
-        <v>58.82</v>
+        <v>65.62</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Taís Nóbrega de Sousa</t>
+          <t>Marina de Moraes Mourão</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>160</v>
+        <v>460</v>
       </c>
       <c r="C27" t="n">
-        <v>260</v>
+        <v>90</v>
       </c>
       <c r="D27" t="n">
-        <v>310</v>
+        <v>390</v>
       </c>
       <c r="E27" t="n">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F27" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="G27" t="n">
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="H27" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I27" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>2090</v>
+        <v>2100</v>
       </c>
       <c r="K27" t="n">
-        <v>65.38</v>
+        <v>19.35</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Edward José de Oliveira</t>
+          <t>Ana Lúcia Teles Rabello</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>110</v>
+        <v>610</v>
       </c>
       <c r="C28" t="n">
+        <v>210</v>
+      </c>
+      <c r="D28" t="n">
+        <v>610</v>
+      </c>
+      <c r="E28" t="n">
+        <v>360</v>
+      </c>
+      <c r="F28" t="n">
         <v>100</v>
       </c>
-      <c r="D28" t="n">
-        <v>380</v>
-      </c>
-      <c r="E28" t="n">
-        <v>395</v>
-      </c>
-      <c r="F28" t="n">
-        <v>230</v>
-      </c>
       <c r="G28" t="n">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="H28" t="n">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1955</v>
+        <v>2090</v>
       </c>
       <c r="K28" t="n">
-        <v>27.27</v>
+        <v>58.82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Luzia Helena Carvalho</t>
+          <t>Edward José de Oliveira</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>250</v>
+        <v>110</v>
       </c>
       <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="n">
+        <v>380</v>
+      </c>
+      <c r="E29" t="n">
+        <v>395</v>
+      </c>
+      <c r="F29" t="n">
+        <v>230</v>
+      </c>
+      <c r="G29" t="n">
         <v>350</v>
       </c>
-      <c r="D29" t="n">
-        <v>170</v>
-      </c>
-      <c r="E29" t="n">
-        <v>360</v>
-      </c>
-      <c r="F29" t="n">
-        <v>410</v>
-      </c>
-      <c r="G29" t="n">
-        <v>260</v>
-      </c>
       <c r="H29" t="n">
-        <v>80</v>
+        <v>390</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1880</v>
+        <v>1955</v>
       </c>
       <c r="K29" t="n">
-        <v>72.73</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Roney Santos Coimbra</t>
+          <t>Luzia Helena Carvalho</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>520</v>
+        <v>250</v>
       </c>
       <c r="C30" t="n">
+        <v>350</v>
+      </c>
+      <c r="D30" t="n">
+        <v>170</v>
+      </c>
+      <c r="E30" t="n">
+        <v>360</v>
+      </c>
+      <c r="F30" t="n">
         <v>410</v>
       </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>170</v>
-      </c>
-      <c r="F30" t="n">
-        <v>160</v>
-      </c>
       <c r="G30" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="H30" t="n">
-        <v>420</v>
+        <v>80</v>
       </c>
       <c r="I30" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>1850</v>
+        <v>1880</v>
       </c>
       <c r="K30" t="n">
-        <v>12.5</v>
+        <v>72.73</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Paulo Marcos Zech Coelho</t>
+          <t>Roney Santos Coimbra</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>375</v>
+        <v>520</v>
       </c>
       <c r="C31" t="n">
-        <v>230</v>
+        <v>410</v>
       </c>
       <c r="D31" t="n">
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="F31" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="G31" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H31" t="n">
-        <v>190</v>
+        <v>420</v>
       </c>
       <c r="I31" t="n">
         <v>80</v>
       </c>
       <c r="J31" t="n">
-        <v>1730</v>
+        <v>1850</v>
       </c>
       <c r="K31" t="n">
-        <v>24.24</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Gustavo Fontes Paz</t>
+          <t>Paulo Marcos Zech Coelho</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>550</v>
+        <v>375</v>
       </c>
       <c r="C32" t="n">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="D32" t="n">
-        <v>170</v>
+        <v>435</v>
       </c>
       <c r="E32" t="n">
         <v>260</v>
       </c>
       <c r="F32" t="n">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="G32" t="n">
-        <v>320</v>
+        <v>20</v>
       </c>
       <c r="H32" t="n">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J32" t="n">
-        <v>1710</v>
+        <v>1730</v>
       </c>
       <c r="K32" t="n">
-        <v>26.09</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Roberta Lima Caldeira</t>
+          <t>Gustavo Fontes Paz</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>310</v>
+        <v>550</v>
       </c>
       <c r="C33" t="n">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="D33" t="n">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E33" t="n">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="F33" t="n">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="G33" t="n">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="H33" t="n">
-        <v>355</v>
+        <v>60</v>
       </c>
       <c r="I33" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>1685</v>
+        <v>1710</v>
       </c>
       <c r="K33" t="n">
-        <v>16.67</v>
+        <v>26.09</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Gustavo Lorenzo</t>
+          <t>Roberta Lima Caldeira</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>180</v>
+        <v>310</v>
       </c>
       <c r="C34" t="n">
+        <v>110</v>
+      </c>
+      <c r="D34" t="n">
         <v>80</v>
       </c>
-      <c r="D34" t="n">
-        <v>170</v>
-      </c>
       <c r="E34" t="n">
-        <v>510</v>
+        <v>280</v>
       </c>
       <c r="F34" t="n">
-        <v>440</v>
+        <v>250</v>
       </c>
       <c r="G34" t="n">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="H34" t="n">
+        <v>355</v>
+      </c>
+      <c r="I34" t="n">
         <v>80</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
       <c r="J34" t="n">
-        <v>1630</v>
+        <v>1685</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Jeronimo Conceição Ruiz</t>
+          <t>Marcelo Gustavo Lorenzo</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>450</v>
+        <v>180</v>
       </c>
       <c r="C35" t="n">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="E35" t="n">
-        <v>410</v>
+        <v>510</v>
       </c>
       <c r="F35" t="n">
-        <v>330</v>
+        <v>440</v>
       </c>
       <c r="G35" t="n">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="H35" t="n">
         <v>80</v>
@@ -1745,457 +1745,457 @@
         <v>1630</v>
       </c>
       <c r="K35" t="n">
-        <v>23.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Caroline Furtado Junqueira</t>
+          <t>Jeronimo Conceição Ruiz</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>170</v>
+        <v>450</v>
       </c>
       <c r="C36" t="n">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E36" t="n">
-        <v>360</v>
+        <v>410</v>
       </c>
       <c r="F36" t="n">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="G36" t="n">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="H36" t="n">
-        <v>450</v>
+        <v>80</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1590</v>
+        <v>1630</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Carlos Eduardo Calzavara Silva</t>
+          <t>Caroline Furtado Junqueira</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="C37" t="n">
-        <v>290</v>
+        <v>170</v>
       </c>
       <c r="D37" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="F37" t="n">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="G37" t="n">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="H37" t="n">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="I37" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1560</v>
+        <v>1590</v>
       </c>
       <c r="K37" t="n">
-        <v>45.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Cristina Toscano Fonseca</t>
+          <t>Carlos Eduardo Calzavara Silva</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="C38" t="n">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="D38" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E38" t="n">
-        <v>80</v>
+        <v>330</v>
       </c>
       <c r="F38" t="n">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="G38" t="n">
-        <v>240</v>
+        <v>350</v>
       </c>
       <c r="H38" t="n">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J38" t="n">
-        <v>1450</v>
+        <v>1560</v>
       </c>
       <c r="K38" t="n">
-        <v>30</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Paloma Helena Fernandes Shimabukuro</t>
+          <t>Cristina Toscano Fonseca</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C39" t="n">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E39" t="n">
-        <v>290</v>
+        <v>80</v>
       </c>
       <c r="F39" t="n">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="G39" t="n">
-        <v>310</v>
+        <v>240</v>
       </c>
       <c r="H39" t="n">
-        <v>310</v>
+        <v>350</v>
       </c>
       <c r="I39" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>1415</v>
+        <v>1450</v>
       </c>
       <c r="K39" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Flora Satiko Kano</t>
+          <t>Paloma Helena Fernandes Shimabukuro</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="C40" t="n">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>290</v>
+      </c>
+      <c r="F40" t="n">
         <v>170</v>
       </c>
-      <c r="E40" t="n">
-        <v>260</v>
-      </c>
-      <c r="F40" t="n">
-        <v>250</v>
-      </c>
       <c r="G40" t="n">
-        <v>180</v>
+        <v>310</v>
       </c>
       <c r="H40" t="n">
-        <v>80</v>
+        <v>310</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J40" t="n">
-        <v>1390</v>
+        <v>1415</v>
       </c>
       <c r="K40" t="n">
-        <v>87.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Lileia Gonçalves Diotaiuti</t>
+          <t>Rita de Cássia Moreira de Souza</t>
         </is>
       </c>
       <c r="B41" t="n">
+        <v>270</v>
+      </c>
+      <c r="C41" t="n">
+        <v>95</v>
+      </c>
+      <c r="D41" t="n">
+        <v>280</v>
+      </c>
+      <c r="E41" t="n">
+        <v>110</v>
+      </c>
+      <c r="F41" t="n">
         <v>400</v>
       </c>
-      <c r="C41" t="n">
-        <v>180</v>
-      </c>
-      <c r="D41" t="n">
-        <v>20</v>
-      </c>
-      <c r="E41" t="n">
-        <v>205</v>
-      </c>
-      <c r="F41" t="n">
-        <v>200</v>
-      </c>
       <c r="G41" t="n">
-        <v>240</v>
+        <v>140</v>
       </c>
       <c r="H41" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>1305</v>
+        <v>1405</v>
       </c>
       <c r="K41" t="n">
-        <v>20</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Rafaella Fortini Grenfell e Queiroz</t>
+          <t>Flora Satiko Kano</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C42" t="n">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="D42" t="n">
-        <v>235</v>
+        <v>170</v>
       </c>
       <c r="E42" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="F42" t="n">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="G42" t="n">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="H42" t="n">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="I42" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>1195</v>
+        <v>1390</v>
       </c>
       <c r="K42" t="n">
-        <v>60.87</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Tânia Maria de Almeida Alves</t>
+          <t>Lileia Gonçalves Diotaiuti</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="C43" t="n">
-        <v>320</v>
+        <v>180</v>
       </c>
       <c r="D43" t="n">
-        <v>210</v>
+        <v>20</v>
       </c>
       <c r="E43" t="n">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="F43" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="G43" t="n">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="H43" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>1185</v>
+        <v>1305</v>
       </c>
       <c r="K43" t="n">
-        <v>31.82</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Érica Alessandra Rocha Alves</t>
+          <t>Rafaella Fortini Grenfell e Queiroz</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="E44" t="n">
-        <v>230</v>
+        <v>90</v>
       </c>
       <c r="F44" t="n">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="G44" t="n">
-        <v>60</v>
+        <v>260</v>
       </c>
       <c r="H44" t="n">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J44" t="n">
-        <v>965</v>
+        <v>1195</v>
       </c>
       <c r="K44" t="n">
-        <v>26.67</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Edelberto Santos Dias</t>
+          <t>Tânia Maria de Almeida Alves</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C45" t="n">
-        <v>170</v>
+        <v>320</v>
       </c>
       <c r="D45" t="n">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E45" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G45" t="n">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="H45" t="n">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>900</v>
+        <v>1185</v>
       </c>
       <c r="K45" t="n">
-        <v>29.41</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Daniel Moreira de Avelar</t>
+          <t>Rosiane Aparecida da Silva Pereira</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D46" t="n">
         <v>190</v>
       </c>
       <c r="E46" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H46" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="J46" t="n">
-        <v>895</v>
+        <v>980</v>
       </c>
       <c r="K46" t="n">
-        <v>52.94</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Alexandre de Magalhaes Vieira Machado</t>
+          <t>Érica Alessandra Rocha Alves</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>380</v>
+        <v>140</v>
       </c>
       <c r="C47" t="n">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="D47" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="F47" t="n">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>875</v>
+        <v>965</v>
       </c>
       <c r="K47" t="n">
-        <v>25</v>
+        <v>26.67</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Erika Michalsky Monteiro</t>
+          <t>Edelberto Santos Dias</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2205,7 +2205,7 @@
         <v>170</v>
       </c>
       <c r="D48" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="E48" t="n">
         <v>130</v>
@@ -2217,200 +2217,311 @@
         <v>80</v>
       </c>
       <c r="H48" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="K48" t="n">
-        <v>42.86</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Carina Margonari de Souza</t>
+          <t>Daniel Moreira de Avelar</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C49" t="n">
+        <v>75</v>
+      </c>
+      <c r="D49" t="n">
+        <v>190</v>
+      </c>
+      <c r="E49" t="n">
         <v>100</v>
       </c>
-      <c r="D49" t="n">
-        <v>60</v>
-      </c>
-      <c r="E49" t="n">
-        <v>80</v>
-      </c>
       <c r="F49" t="n">
-        <v>310</v>
+        <v>170</v>
       </c>
       <c r="G49" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="H49" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>790</v>
+        <v>895</v>
       </c>
       <c r="K49" t="n">
-        <v>25</v>
+        <v>52.94</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Álvaro Gil Araújo Ferreira</t>
+          <t>Alexandre de Magalhaes Vieira Machado</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="C50" t="n">
+        <v>85</v>
+      </c>
+      <c r="D50" t="n">
+        <v>150</v>
+      </c>
+      <c r="E50" t="n">
         <v>90</v>
       </c>
-      <c r="D50" t="n">
-        <v>40</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>170</v>
       </c>
-      <c r="F50" t="n">
-        <v>250</v>
-      </c>
       <c r="G50" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>790</v>
+        <v>875</v>
       </c>
       <c r="K50" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Jaquelline Germano de Oliveira</t>
+          <t>Erika Michalsky Monteiro</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C51" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D51" t="n">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="E51" t="n">
-        <v>290</v>
+        <v>130</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I51" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>730</v>
+        <v>800</v>
       </c>
       <c r="K51" t="n">
-        <v>28.57</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Soraya Torres Gaze Jangola</t>
+          <t>Carina Margonari de Souza</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C52" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E52" t="n">
         <v>80</v>
       </c>
       <c r="F52" t="n">
-        <v>175</v>
+        <v>310</v>
       </c>
       <c r="G52" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H52" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>540</v>
+        <v>790</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
+          <t>Álvaro Gil Araújo Ferreira</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>90</v>
+      </c>
+      <c r="D53" t="n">
+        <v>40</v>
+      </c>
+      <c r="E53" t="n">
+        <v>170</v>
+      </c>
+      <c r="F53" t="n">
+        <v>250</v>
+      </c>
+      <c r="G53" t="n">
+        <v>60</v>
+      </c>
+      <c r="H53" t="n">
+        <v>180</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>790</v>
+      </c>
+      <c r="K53" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Jaquelline Germano de Oliveira</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>160</v>
+      </c>
+      <c r="D54" t="n">
+        <v>60</v>
+      </c>
+      <c r="E54" t="n">
+        <v>290</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>140</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>80</v>
+      </c>
+      <c r="J54" t="n">
+        <v>730</v>
+      </c>
+      <c r="K54" t="n">
+        <v>28.57</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>Soraya Torres Gaze Jangola</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>95</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>80</v>
+      </c>
+      <c r="F55" t="n">
+        <v>175</v>
+      </c>
+      <c r="G55" t="n">
+        <v>100</v>
+      </c>
+      <c r="H55" t="n">
+        <v>180</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>630</v>
+      </c>
+      <c r="K55" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
           <t>Marco Antônio da Silva Campos</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="B56" t="n">
         <v>60</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C56" t="n">
         <v>95</v>
       </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
         <v>100</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F56" t="n">
         <v>140</v>
       </c>
-      <c r="G53" t="n">
+      <c r="G56" t="n">
         <v>20</v>
       </c>
-      <c r="H53" t="n">
+      <c r="H56" t="n">
         <v>80</v>
       </c>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="n">
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
         <v>495</v>
       </c>
-      <c r="K53" t="n">
+      <c r="K56" t="n">
         <v>23.08</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Melhoria na implementação da extração
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,13 +555,13 @@
         <v>1610</v>
       </c>
       <c r="I3" t="n">
-        <v>805</v>
+        <v>435</v>
       </c>
       <c r="J3" t="n">
-        <v>9225</v>
+        <v>8855</v>
       </c>
       <c r="K3" t="n">
-        <v>11.11</v>
+        <v>11.63</v>
       </c>
     </row>
     <row r="4">
@@ -703,124 +703,124 @@
         <v>290</v>
       </c>
       <c r="I7" t="n">
-        <v>470</v>
+        <v>380</v>
       </c>
       <c r="J7" t="n">
-        <v>3845</v>
+        <v>3755</v>
       </c>
       <c r="K7" t="n">
-        <v>57.89</v>
+        <v>57.14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Pedro Pinto Soares</t>
+          <t>Lis Ribeiro do Valle Antonelli</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>540</v>
+        <v>310</v>
       </c>
       <c r="C8" t="n">
-        <v>560</v>
+        <v>630</v>
       </c>
       <c r="D8" t="n">
-        <v>620</v>
+        <v>690</v>
       </c>
       <c r="E8" t="n">
-        <v>520</v>
+        <v>470</v>
       </c>
       <c r="F8" t="n">
-        <v>750</v>
+        <v>670</v>
       </c>
       <c r="G8" t="n">
-        <v>150</v>
+        <v>530</v>
       </c>
       <c r="H8" t="n">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="I8" t="n">
-        <v>350</v>
+        <v>90</v>
       </c>
       <c r="J8" t="n">
-        <v>3710</v>
+        <v>3660</v>
       </c>
       <c r="K8" t="n">
-        <v>10.34</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Lis Ribeiro do Valle Antonelli</t>
+          <t>Rodrigo Correa de Oliveira</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>310</v>
+        <v>1290</v>
       </c>
       <c r="C9" t="n">
-        <v>630</v>
+        <v>360</v>
       </c>
       <c r="D9" t="n">
-        <v>690</v>
+        <v>770</v>
       </c>
       <c r="E9" t="n">
-        <v>470</v>
+        <v>360</v>
       </c>
       <c r="F9" t="n">
-        <v>670</v>
+        <v>360</v>
       </c>
       <c r="G9" t="n">
-        <v>530</v>
+        <v>230</v>
       </c>
       <c r="H9" t="n">
         <v>270</v>
       </c>
       <c r="I9" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>3660</v>
+        <v>3640</v>
       </c>
       <c r="K9" t="n">
-        <v>14.89</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Correa de Oliveira</t>
+          <t>Rodrigo Pedro Pinto Soares</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1290</v>
+        <v>540</v>
       </c>
       <c r="C10" t="n">
-        <v>360</v>
+        <v>560</v>
       </c>
       <c r="D10" t="n">
-        <v>770</v>
+        <v>620</v>
       </c>
       <c r="E10" t="n">
-        <v>360</v>
+        <v>520</v>
       </c>
       <c r="F10" t="n">
-        <v>360</v>
+        <v>750</v>
       </c>
       <c r="G10" t="n">
-        <v>230</v>
+        <v>150</v>
       </c>
       <c r="H10" t="n">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="J10" t="n">
-        <v>3640</v>
+        <v>3620</v>
       </c>
       <c r="K10" t="n">
-        <v>8.33</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="11">
@@ -937,75 +937,75 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Celia Maria Ferreira Gontijo</t>
+          <t>Antonio Mauro Rezende</t>
         </is>
       </c>
       <c r="B14" t="n">
+        <v>230</v>
+      </c>
+      <c r="C14" t="n">
+        <v>360</v>
+      </c>
+      <c r="D14" t="n">
         <v>480</v>
       </c>
-      <c r="C14" t="n">
-        <v>585</v>
-      </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
+        <v>560</v>
+      </c>
+      <c r="F14" t="n">
+        <v>450</v>
+      </c>
+      <c r="G14" t="n">
+        <v>280</v>
+      </c>
+      <c r="H14" t="n">
         <v>390</v>
       </c>
-      <c r="E14" t="n">
-        <v>500</v>
-      </c>
-      <c r="F14" t="n">
-        <v>260</v>
-      </c>
-      <c r="G14" t="n">
-        <v>270</v>
-      </c>
-      <c r="H14" t="n">
-        <v>260</v>
-      </c>
       <c r="I14" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="J14" t="n">
-        <v>2785</v>
+        <v>2765</v>
       </c>
       <c r="K14" t="n">
-        <v>19.51</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Antonio Mauro Rezende</t>
+          <t>Celia Maria Ferreira Gontijo</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>230</v>
+        <v>480</v>
       </c>
       <c r="C15" t="n">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="D15" t="n">
-        <v>480</v>
+        <v>390</v>
       </c>
       <c r="E15" t="n">
-        <v>560</v>
+        <v>500</v>
       </c>
       <c r="F15" t="n">
-        <v>450</v>
+        <v>260</v>
       </c>
       <c r="G15" t="n">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="H15" t="n">
-        <v>390</v>
+        <v>260</v>
       </c>
       <c r="I15" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>2765</v>
+        <v>2745</v>
       </c>
       <c r="K15" t="n">
-        <v>7.14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -1159,581 +1159,581 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Márcio Sobreira Silva Araújo</t>
+          <t>Cristiana Ferreira Alves de Brito</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>145</v>
+        <v>370</v>
       </c>
       <c r="C20" t="n">
-        <v>665</v>
+        <v>440</v>
       </c>
       <c r="D20" t="n">
-        <v>180</v>
+        <v>530</v>
       </c>
       <c r="E20" t="n">
-        <v>215</v>
+        <v>270</v>
       </c>
       <c r="F20" t="n">
-        <v>185</v>
+        <v>330</v>
       </c>
       <c r="G20" t="n">
-        <v>475</v>
+        <v>160</v>
       </c>
       <c r="H20" t="n">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="I20" t="n">
-        <v>380</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>2285</v>
+        <v>2270</v>
       </c>
       <c r="K20" t="n">
-        <v>25</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Cristiana Ferreira Alves de Brito</t>
+          <t>Alessandra Aparecida Guarneri</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="C21" t="n">
-        <v>440</v>
+        <v>220</v>
       </c>
       <c r="D21" t="n">
-        <v>530</v>
+        <v>210</v>
       </c>
       <c r="E21" t="n">
-        <v>270</v>
+        <v>430</v>
       </c>
       <c r="F21" t="n">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="G21" t="n">
-        <v>160</v>
+        <v>260</v>
       </c>
       <c r="H21" t="n">
-        <v>170</v>
+        <v>360</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J21" t="n">
-        <v>2270</v>
+        <v>2260</v>
       </c>
       <c r="K21" t="n">
-        <v>43.75</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Alessandra Aparecida Guarneri</t>
+          <t>Marcelo Antonio Pascoal Xavier</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>350</v>
+        <v>225</v>
       </c>
       <c r="C22" t="n">
-        <v>220</v>
+        <v>545</v>
       </c>
       <c r="D22" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="F22" t="n">
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="G22" t="n">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="H22" t="n">
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="I22" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="J22" t="n">
-        <v>2260</v>
+        <v>2145</v>
       </c>
       <c r="K22" t="n">
-        <v>22.22</v>
+        <v>30.56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Antonio Pascoal Xavier</t>
+          <t>Márcio Sobreira Silva Araújo</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="C23" t="n">
-        <v>545</v>
+        <v>665</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E23" t="n">
-        <v>435</v>
+        <v>215</v>
       </c>
       <c r="F23" t="n">
-        <v>370</v>
+        <v>185</v>
       </c>
       <c r="G23" t="n">
-        <v>200</v>
+        <v>475</v>
       </c>
       <c r="H23" t="n">
-        <v>240</v>
+        <v>40</v>
       </c>
       <c r="I23" t="n">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="J23" t="n">
-        <v>2145</v>
+        <v>2125</v>
       </c>
       <c r="K23" t="n">
-        <v>30.56</v>
+        <v>23.53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Taís Nóbrega de Sousa</t>
+          <t>Rubens Lima do Monte Neto</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="C24" t="n">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="D24" t="n">
-        <v>310</v>
+        <v>40</v>
       </c>
       <c r="E24" t="n">
-        <v>350</v>
+        <v>280</v>
       </c>
       <c r="F24" t="n">
-        <v>320</v>
+        <v>420</v>
       </c>
       <c r="G24" t="n">
-        <v>350</v>
+        <v>425</v>
       </c>
       <c r="H24" t="n">
-        <v>160</v>
+        <v>330</v>
       </c>
       <c r="I24" t="n">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="J24" t="n">
-        <v>2130</v>
+        <v>2105</v>
       </c>
       <c r="K24" t="n">
-        <v>62.96</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Rubens Lima do Monte Neto</t>
+          <t>Marina de Moraes Mourão</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>80</v>
+        <v>460</v>
       </c>
       <c r="C25" t="n">
-        <v>400</v>
+        <v>90</v>
       </c>
       <c r="D25" t="n">
-        <v>40</v>
+        <v>390</v>
       </c>
       <c r="E25" t="n">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="F25" t="n">
-        <v>420</v>
+        <v>220</v>
       </c>
       <c r="G25" t="n">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="H25" t="n">
-        <v>330</v>
+        <v>200</v>
       </c>
       <c r="I25" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>2105</v>
+        <v>2100</v>
       </c>
       <c r="K25" t="n">
-        <v>17.65</v>
+        <v>19.35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Pedro Augusto Alves</t>
+          <t>Ana Lúcia Teles Rabello</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>610</v>
       </c>
       <c r="C26" t="n">
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="D26" t="n">
-        <v>250</v>
+        <v>610</v>
       </c>
       <c r="E26" t="n">
-        <v>440</v>
+        <v>360</v>
       </c>
       <c r="F26" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G26" t="n">
-        <v>460</v>
+        <v>180</v>
       </c>
       <c r="H26" t="n">
-        <v>380</v>
+        <v>20</v>
       </c>
       <c r="I26" t="n">
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>2105</v>
+        <v>2090</v>
       </c>
       <c r="K26" t="n">
-        <v>65.62</v>
+        <v>58.82</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Marina de Moraes Mourão</t>
+          <t>Taís Nóbrega de Sousa</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>460</v>
+        <v>160</v>
       </c>
       <c r="C27" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="D27" t="n">
-        <v>390</v>
+        <v>310</v>
       </c>
       <c r="E27" t="n">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="F27" t="n">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="G27" t="n">
-        <v>410</v>
+        <v>350</v>
       </c>
       <c r="H27" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="J27" t="n">
-        <v>2100</v>
+        <v>2090</v>
       </c>
       <c r="K27" t="n">
-        <v>19.35</v>
+        <v>65.38</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Ana Lúcia Teles Rabello</t>
+          <t>Edward José de Oliveira</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>610</v>
+        <v>110</v>
       </c>
       <c r="C28" t="n">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="D28" t="n">
-        <v>610</v>
+        <v>380</v>
       </c>
       <c r="E28" t="n">
-        <v>360</v>
+        <v>395</v>
       </c>
       <c r="F28" t="n">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="G28" t="n">
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="H28" t="n">
-        <v>20</v>
+        <v>390</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>2090</v>
+        <v>1955</v>
       </c>
       <c r="K28" t="n">
-        <v>58.82</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Edward José de Oliveira</t>
+          <t>Luzia Helena Carvalho</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>110</v>
+        <v>250</v>
       </c>
       <c r="C29" t="n">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="D29" t="n">
-        <v>380</v>
+        <v>170</v>
       </c>
       <c r="E29" t="n">
-        <v>395</v>
+        <v>360</v>
       </c>
       <c r="F29" t="n">
-        <v>230</v>
+        <v>410</v>
       </c>
       <c r="G29" t="n">
-        <v>350</v>
+        <v>260</v>
       </c>
       <c r="H29" t="n">
-        <v>390</v>
+        <v>80</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1955</v>
+        <v>1880</v>
       </c>
       <c r="K29" t="n">
-        <v>27.27</v>
+        <v>72.73</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Luzia Helena Carvalho</t>
+          <t>Roney Santos Coimbra</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>250</v>
+        <v>520</v>
       </c>
       <c r="C30" t="n">
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
         <v>170</v>
       </c>
-      <c r="E30" t="n">
-        <v>360</v>
-      </c>
       <c r="F30" t="n">
-        <v>410</v>
+        <v>160</v>
       </c>
       <c r="G30" t="n">
-        <v>260</v>
+        <v>90</v>
       </c>
       <c r="H30" t="n">
+        <v>420</v>
+      </c>
+      <c r="I30" t="n">
         <v>80</v>
       </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
       <c r="J30" t="n">
-        <v>1880</v>
+        <v>1850</v>
       </c>
       <c r="K30" t="n">
-        <v>72.73</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Roney Santos Coimbra</t>
+          <t>Paulo Marcos Zech Coelho</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>520</v>
+        <v>375</v>
       </c>
       <c r="C31" t="n">
-        <v>410</v>
+        <v>230</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="E31" t="n">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="F31" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G31" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="H31" t="n">
-        <v>420</v>
+        <v>190</v>
       </c>
       <c r="I31" t="n">
         <v>80</v>
       </c>
       <c r="J31" t="n">
-        <v>1850</v>
+        <v>1730</v>
       </c>
       <c r="K31" t="n">
-        <v>12.5</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Paulo Marcos Zech Coelho</t>
+          <t>Gustavo Fontes Paz</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>375</v>
+        <v>550</v>
       </c>
       <c r="C32" t="n">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="D32" t="n">
-        <v>435</v>
+        <v>170</v>
       </c>
       <c r="E32" t="n">
         <v>260</v>
       </c>
       <c r="F32" t="n">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="G32" t="n">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="H32" t="n">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="I32" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>1730</v>
+        <v>1710</v>
       </c>
       <c r="K32" t="n">
-        <v>24.24</v>
+        <v>26.09</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Gustavo Fontes Paz</t>
+          <t>Roberta Lima Caldeira</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>550</v>
+        <v>310</v>
       </c>
       <c r="C33" t="n">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D33" t="n">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="E33" t="n">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="F33" t="n">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="G33" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="H33" t="n">
-        <v>60</v>
+        <v>355</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J33" t="n">
-        <v>1710</v>
+        <v>1685</v>
       </c>
       <c r="K33" t="n">
-        <v>26.09</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Roberta Lima Caldeira</t>
+          <t>Marcelo Gustavo Lorenzo</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>310</v>
+        <v>180</v>
       </c>
       <c r="C34" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D34" t="n">
+        <v>170</v>
+      </c>
+      <c r="E34" t="n">
+        <v>510</v>
+      </c>
+      <c r="F34" t="n">
+        <v>440</v>
+      </c>
+      <c r="G34" t="n">
+        <v>170</v>
+      </c>
+      <c r="H34" t="n">
         <v>80</v>
       </c>
-      <c r="E34" t="n">
-        <v>280</v>
-      </c>
-      <c r="F34" t="n">
-        <v>250</v>
-      </c>
-      <c r="G34" t="n">
-        <v>220</v>
-      </c>
-      <c r="H34" t="n">
-        <v>355</v>
-      </c>
       <c r="I34" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>1685</v>
+        <v>1630</v>
       </c>
       <c r="K34" t="n">
-        <v>16.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Gustavo Lorenzo</t>
+          <t>Jeronimo Conceição Ruiz</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>180</v>
+        <v>450</v>
       </c>
       <c r="C35" t="n">
+        <v>220</v>
+      </c>
+      <c r="D35" t="n">
+        <v>60</v>
+      </c>
+      <c r="E35" t="n">
+        <v>410</v>
+      </c>
+      <c r="F35" t="n">
+        <v>330</v>
+      </c>
+      <c r="G35" t="n">
         <v>80</v>
-      </c>
-      <c r="D35" t="n">
-        <v>170</v>
-      </c>
-      <c r="E35" t="n">
-        <v>510</v>
-      </c>
-      <c r="F35" t="n">
-        <v>440</v>
-      </c>
-      <c r="G35" t="n">
-        <v>170</v>
       </c>
       <c r="H35" t="n">
         <v>80</v>
@@ -1745,457 +1745,457 @@
         <v>1630</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Jeronimo Conceição Ruiz</t>
+          <t>Caroline Furtado Junqueira</t>
         </is>
       </c>
       <c r="B36" t="n">
+        <v>170</v>
+      </c>
+      <c r="C36" t="n">
+        <v>170</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>360</v>
+      </c>
+      <c r="F36" t="n">
+        <v>240</v>
+      </c>
+      <c r="G36" t="n">
+        <v>200</v>
+      </c>
+      <c r="H36" t="n">
         <v>450</v>
       </c>
-      <c r="C36" t="n">
-        <v>220</v>
-      </c>
-      <c r="D36" t="n">
-        <v>60</v>
-      </c>
-      <c r="E36" t="n">
-        <v>410</v>
-      </c>
-      <c r="F36" t="n">
-        <v>330</v>
-      </c>
-      <c r="G36" t="n">
-        <v>80</v>
-      </c>
-      <c r="H36" t="n">
-        <v>80</v>
-      </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1630</v>
+        <v>1590</v>
       </c>
       <c r="K36" t="n">
-        <v>23.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Caroline Furtado Junqueira</t>
+          <t>Carlos Eduardo Calzavara Silva</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="C37" t="n">
-        <v>170</v>
+        <v>290</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E37" t="n">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="F37" t="n">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="G37" t="n">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="H37" t="n">
-        <v>450</v>
+        <v>330</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J37" t="n">
-        <v>1590</v>
+        <v>1560</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Carlos Eduardo Calzavara Silva</t>
+          <t>Cristina Toscano Fonseca</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="C38" t="n">
-        <v>290</v>
+        <v>210</v>
       </c>
       <c r="D38" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="E38" t="n">
-        <v>330</v>
+        <v>80</v>
       </c>
       <c r="F38" t="n">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="G38" t="n">
+        <v>240</v>
+      </c>
+      <c r="H38" t="n">
         <v>350</v>
       </c>
-      <c r="H38" t="n">
-        <v>330</v>
-      </c>
       <c r="I38" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>1560</v>
+        <v>1450</v>
       </c>
       <c r="K38" t="n">
-        <v>45.45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Cristina Toscano Fonseca</t>
+          <t>Paloma Helena Fernandes Shimabukuro</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C39" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="D39" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>80</v>
+        <v>290</v>
       </c>
       <c r="F39" t="n">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="G39" t="n">
-        <v>240</v>
+        <v>310</v>
       </c>
       <c r="H39" t="n">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J39" t="n">
-        <v>1450</v>
+        <v>1415</v>
       </c>
       <c r="K39" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Paloma Helena Fernandes Shimabukuro</t>
+          <t>Flora Satiko Kano</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C40" t="n">
+        <v>270</v>
+      </c>
+      <c r="D40" t="n">
         <v>170</v>
       </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
       <c r="E40" t="n">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="F40" t="n">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="G40" t="n">
-        <v>310</v>
+        <v>180</v>
       </c>
       <c r="H40" t="n">
-        <v>310</v>
+        <v>80</v>
       </c>
       <c r="I40" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>1415</v>
+        <v>1390</v>
       </c>
       <c r="K40" t="n">
-        <v>16</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Rita de Cássia Moreira de Souza</t>
+          <t>Lileia Gonçalves Diotaiuti</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>270</v>
+        <v>400</v>
       </c>
       <c r="C41" t="n">
-        <v>95</v>
+        <v>180</v>
       </c>
       <c r="D41" t="n">
-        <v>280</v>
+        <v>20</v>
       </c>
       <c r="E41" t="n">
-        <v>110</v>
+        <v>205</v>
       </c>
       <c r="F41" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G41" t="n">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="H41" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>1405</v>
+        <v>1305</v>
       </c>
       <c r="K41" t="n">
-        <v>4.35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Flora Satiko Kano</t>
+          <t>Rafaella Fortini Grenfell e Queiroz</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>270</v>
+        <v>60</v>
       </c>
       <c r="D42" t="n">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="E42" t="n">
+        <v>90</v>
+      </c>
+      <c r="F42" t="n">
+        <v>220</v>
+      </c>
+      <c r="G42" t="n">
         <v>260</v>
       </c>
-      <c r="F42" t="n">
+      <c r="H42" t="n">
         <v>250</v>
       </c>
-      <c r="G42" t="n">
-        <v>180</v>
-      </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>80</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
       <c r="J42" t="n">
-        <v>1390</v>
+        <v>1195</v>
       </c>
       <c r="K42" t="n">
-        <v>87.5</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Lileia Gonçalves Diotaiuti</t>
+          <t>Tânia Maria de Almeida Alves</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="C43" t="n">
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="D43" t="n">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="E43" t="n">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="F43" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="G43" t="n">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="H43" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>1305</v>
+        <v>1185</v>
       </c>
       <c r="K43" t="n">
-        <v>20</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Rafaella Fortini Grenfell e Queiroz</t>
+          <t>Érica Alessandra Rocha Alves</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C44" t="n">
+        <v>165</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>230</v>
+      </c>
+      <c r="F44" t="n">
+        <v>100</v>
+      </c>
+      <c r="G44" t="n">
         <v>60</v>
       </c>
-      <c r="D44" t="n">
-        <v>235</v>
-      </c>
-      <c r="E44" t="n">
-        <v>90</v>
-      </c>
-      <c r="F44" t="n">
-        <v>220</v>
-      </c>
-      <c r="G44" t="n">
-        <v>260</v>
-      </c>
       <c r="H44" t="n">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="I44" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>1195</v>
+        <v>965</v>
       </c>
       <c r="K44" t="n">
-        <v>60.87</v>
+        <v>26.67</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Tânia Maria de Almeida Alves</t>
+          <t>Edelberto Santos Dias</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C45" t="n">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="D45" t="n">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="E45" t="n">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="F45" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="H45" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>1185</v>
+        <v>900</v>
       </c>
       <c r="K45" t="n">
-        <v>31.82</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Rosiane Aparecida da Silva Pereira</t>
+          <t>Daniel Moreira de Avelar</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C46" t="n">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D46" t="n">
         <v>190</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="G46" t="n">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="H46" t="n">
-        <v>260</v>
+        <v>90</v>
       </c>
       <c r="I46" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>980</v>
+        <v>895</v>
       </c>
       <c r="K46" t="n">
-        <v>28.57</v>
+        <v>52.94</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Érica Alessandra Rocha Alves</t>
+          <t>Alexandre de Magalhaes Vieira Machado</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>140</v>
+        <v>380</v>
       </c>
       <c r="C47" t="n">
-        <v>165</v>
+        <v>85</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E47" t="n">
-        <v>230</v>
+        <v>90</v>
       </c>
       <c r="F47" t="n">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="G47" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>965</v>
+        <v>875</v>
       </c>
       <c r="K47" t="n">
-        <v>26.67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Edelberto Santos Dias</t>
+          <t>Erika Michalsky Monteiro</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2205,7 +2205,7 @@
         <v>170</v>
       </c>
       <c r="D48" t="n">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E48" t="n">
         <v>130</v>
@@ -2217,311 +2217,200 @@
         <v>80</v>
       </c>
       <c r="H48" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="K48" t="n">
-        <v>29.41</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Daniel Moreira de Avelar</t>
+          <t>Carina Margonari de Souza</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C49" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D49" t="n">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="E49" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F49" t="n">
-        <v>170</v>
+        <v>310</v>
       </c>
       <c r="G49" t="n">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="H49" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>895</v>
+        <v>790</v>
       </c>
       <c r="K49" t="n">
-        <v>52.94</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Alexandre de Magalhaes Vieira Machado</t>
+          <t>Álvaro Gil Araújo Ferreira</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>380</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D50" t="n">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="E50" t="n">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="F50" t="n">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>875</v>
+        <v>790</v>
       </c>
       <c r="K50" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Erika Michalsky Monteiro</t>
+          <t>Jaquelline Germano de Oliveira</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D51" t="n">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="E51" t="n">
-        <v>130</v>
+        <v>290</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
+        <v>140</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
         <v>80</v>
       </c>
-      <c r="H51" t="n">
-        <v>120</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
       <c r="J51" t="n">
-        <v>800</v>
+        <v>730</v>
       </c>
       <c r="K51" t="n">
-        <v>42.86</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Carina Margonari de Souza</t>
+          <t>Soraya Torres Gaze Jangola</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D52" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>80</v>
       </c>
       <c r="F52" t="n">
-        <v>310</v>
+        <v>175</v>
       </c>
       <c r="G52" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H52" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>790</v>
+        <v>540</v>
       </c>
       <c r="K52" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Álvaro Gil Araújo Ferreira</t>
+          <t>Marco Antônio da Silva Campos</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C53" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D53" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="F53" t="n">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="G53" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H53" t="n">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>790</v>
+        <v>495</v>
       </c>
       <c r="K53" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Jaquelline Germano de Oliveira</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>160</v>
-      </c>
-      <c r="D54" t="n">
-        <v>60</v>
-      </c>
-      <c r="E54" t="n">
-        <v>290</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>140</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>80</v>
-      </c>
-      <c r="J54" t="n">
-        <v>730</v>
-      </c>
-      <c r="K54" t="n">
-        <v>28.57</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Soraya Torres Gaze Jangola</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" t="n">
-        <v>95</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" t="n">
-        <v>80</v>
-      </c>
-      <c r="F55" t="n">
-        <v>175</v>
-      </c>
-      <c r="G55" t="n">
-        <v>100</v>
-      </c>
-      <c r="H55" t="n">
-        <v>180</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>630</v>
-      </c>
-      <c r="K55" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Marco Antônio da Silva Campos</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>60</v>
-      </c>
-      <c r="C56" t="n">
-        <v>95</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" t="n">
-        <v>100</v>
-      </c>
-      <c r="F56" t="n">
-        <v>140</v>
-      </c>
-      <c r="G56" t="n">
-        <v>20</v>
-      </c>
-      <c r="H56" t="n">
-        <v>80</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
-        <v>495</v>
-      </c>
-      <c r="K56" t="n">
         <v>23.08</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção da persistência dados discentes
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,13 +555,13 @@
         <v>1610</v>
       </c>
       <c r="I3" t="n">
-        <v>435</v>
+        <v>805</v>
       </c>
       <c r="J3" t="n">
-        <v>8855</v>
+        <v>9225</v>
       </c>
       <c r="K3" t="n">
-        <v>11.63</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="4">
@@ -703,124 +703,124 @@
         <v>290</v>
       </c>
       <c r="I7" t="n">
-        <v>380</v>
+        <v>470</v>
       </c>
       <c r="J7" t="n">
-        <v>3755</v>
+        <v>3845</v>
       </c>
       <c r="K7" t="n">
-        <v>57.14</v>
+        <v>57.89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Lis Ribeiro do Valle Antonelli</t>
+          <t>Rodrigo Pedro Pinto Soares</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>310</v>
+        <v>540</v>
       </c>
       <c r="C8" t="n">
-        <v>630</v>
+        <v>560</v>
       </c>
       <c r="D8" t="n">
-        <v>690</v>
+        <v>620</v>
       </c>
       <c r="E8" t="n">
-        <v>470</v>
+        <v>520</v>
       </c>
       <c r="F8" t="n">
-        <v>670</v>
+        <v>750</v>
       </c>
       <c r="G8" t="n">
-        <v>530</v>
+        <v>150</v>
       </c>
       <c r="H8" t="n">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="I8" t="n">
-        <v>90</v>
+        <v>350</v>
       </c>
       <c r="J8" t="n">
-        <v>3660</v>
+        <v>3710</v>
       </c>
       <c r="K8" t="n">
-        <v>14.89</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Correa de Oliveira</t>
+          <t>Lis Ribeiro do Valle Antonelli</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1290</v>
+        <v>310</v>
       </c>
       <c r="C9" t="n">
-        <v>360</v>
+        <v>630</v>
       </c>
       <c r="D9" t="n">
-        <v>770</v>
+        <v>690</v>
       </c>
       <c r="E9" t="n">
-        <v>360</v>
+        <v>470</v>
       </c>
       <c r="F9" t="n">
-        <v>360</v>
+        <v>670</v>
       </c>
       <c r="G9" t="n">
-        <v>230</v>
+        <v>530</v>
       </c>
       <c r="H9" t="n">
         <v>270</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J9" t="n">
-        <v>3640</v>
+        <v>3660</v>
       </c>
       <c r="K9" t="n">
-        <v>8.33</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Rodrigo Pedro Pinto Soares</t>
+          <t>Rodrigo Correa de Oliveira</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>540</v>
+        <v>1290</v>
       </c>
       <c r="C10" t="n">
-        <v>560</v>
+        <v>360</v>
       </c>
       <c r="D10" t="n">
-        <v>620</v>
+        <v>770</v>
       </c>
       <c r="E10" t="n">
-        <v>520</v>
+        <v>360</v>
       </c>
       <c r="F10" t="n">
-        <v>750</v>
+        <v>360</v>
       </c>
       <c r="G10" t="n">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="H10" t="n">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="I10" t="n">
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>3620</v>
+        <v>3640</v>
       </c>
       <c r="K10" t="n">
-        <v>10.53</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="11">
@@ -937,75 +937,75 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Antonio Mauro Rezende</t>
+          <t>Celia Maria Ferreira Gontijo</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>230</v>
+        <v>480</v>
       </c>
       <c r="C14" t="n">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="D14" t="n">
-        <v>480</v>
+        <v>390</v>
       </c>
       <c r="E14" t="n">
-        <v>560</v>
+        <v>500</v>
       </c>
       <c r="F14" t="n">
-        <v>450</v>
+        <v>260</v>
       </c>
       <c r="G14" t="n">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="H14" t="n">
-        <v>390</v>
+        <v>260</v>
       </c>
       <c r="I14" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="J14" t="n">
-        <v>2765</v>
+        <v>2785</v>
       </c>
       <c r="K14" t="n">
-        <v>7.14</v>
+        <v>19.51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Celia Maria Ferreira Gontijo</t>
+          <t>Antonio Mauro Rezende</t>
         </is>
       </c>
       <c r="B15" t="n">
+        <v>230</v>
+      </c>
+      <c r="C15" t="n">
+        <v>360</v>
+      </c>
+      <c r="D15" t="n">
         <v>480</v>
       </c>
-      <c r="C15" t="n">
-        <v>585</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>560</v>
+      </c>
+      <c r="F15" t="n">
+        <v>450</v>
+      </c>
+      <c r="G15" t="n">
+        <v>280</v>
+      </c>
+      <c r="H15" t="n">
         <v>390</v>
       </c>
-      <c r="E15" t="n">
-        <v>500</v>
-      </c>
-      <c r="F15" t="n">
-        <v>260</v>
-      </c>
-      <c r="G15" t="n">
-        <v>270</v>
-      </c>
-      <c r="H15" t="n">
-        <v>260</v>
-      </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J15" t="n">
-        <v>2745</v>
+        <v>2765</v>
       </c>
       <c r="K15" t="n">
-        <v>20</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="16">
@@ -1159,581 +1159,581 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Cristiana Ferreira Alves de Brito</t>
+          <t>Márcio Sobreira Silva Araújo</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>370</v>
+        <v>145</v>
       </c>
       <c r="C20" t="n">
-        <v>440</v>
+        <v>665</v>
       </c>
       <c r="D20" t="n">
-        <v>530</v>
+        <v>180</v>
       </c>
       <c r="E20" t="n">
-        <v>270</v>
+        <v>215</v>
       </c>
       <c r="F20" t="n">
-        <v>330</v>
+        <v>185</v>
       </c>
       <c r="G20" t="n">
-        <v>160</v>
+        <v>475</v>
       </c>
       <c r="H20" t="n">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="J20" t="n">
-        <v>2270</v>
+        <v>2285</v>
       </c>
       <c r="K20" t="n">
-        <v>43.75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Alessandra Aparecida Guarneri</t>
+          <t>Cristiana Ferreira Alves de Brito</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C21" t="n">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="D21" t="n">
-        <v>210</v>
+        <v>530</v>
       </c>
       <c r="E21" t="n">
-        <v>430</v>
+        <v>270</v>
       </c>
       <c r="F21" t="n">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="G21" t="n">
-        <v>260</v>
+        <v>160</v>
       </c>
       <c r="H21" t="n">
-        <v>360</v>
+        <v>170</v>
       </c>
       <c r="I21" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>2260</v>
+        <v>2270</v>
       </c>
       <c r="K21" t="n">
-        <v>22.22</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Antonio Pascoal Xavier</t>
+          <t>Alessandra Aparecida Guarneri</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="C22" t="n">
-        <v>545</v>
+        <v>220</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="E22" t="n">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F22" t="n">
-        <v>370</v>
+        <v>340</v>
       </c>
       <c r="G22" t="n">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="H22" t="n">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="I22" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="J22" t="n">
-        <v>2145</v>
+        <v>2260</v>
       </c>
       <c r="K22" t="n">
-        <v>30.56</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Márcio Sobreira Silva Araújo</t>
+          <t>Marcelo Antonio Pascoal Xavier</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="C23" t="n">
-        <v>665</v>
+        <v>545</v>
       </c>
       <c r="D23" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>215</v>
+        <v>435</v>
       </c>
       <c r="F23" t="n">
-        <v>185</v>
+        <v>370</v>
       </c>
       <c r="G23" t="n">
-        <v>475</v>
+        <v>200</v>
       </c>
       <c r="H23" t="n">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="I23" t="n">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="J23" t="n">
-        <v>2125</v>
+        <v>2145</v>
       </c>
       <c r="K23" t="n">
-        <v>23.53</v>
+        <v>30.56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Rubens Lima do Monte Neto</t>
+          <t>Taís Nóbrega de Sousa</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="C24" t="n">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="D24" t="n">
-        <v>40</v>
+        <v>310</v>
       </c>
       <c r="E24" t="n">
-        <v>280</v>
+        <v>350</v>
       </c>
       <c r="F24" t="n">
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="G24" t="n">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="H24" t="n">
-        <v>330</v>
+        <v>160</v>
       </c>
       <c r="I24" t="n">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="J24" t="n">
-        <v>2105</v>
+        <v>2130</v>
       </c>
       <c r="K24" t="n">
-        <v>17.65</v>
+        <v>62.96</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Marina de Moraes Mourão</t>
+          <t>Rubens Lima do Monte Neto</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>460</v>
+        <v>80</v>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>400</v>
       </c>
       <c r="D25" t="n">
-        <v>390</v>
+        <v>40</v>
       </c>
       <c r="E25" t="n">
+        <v>280</v>
+      </c>
+      <c r="F25" t="n">
+        <v>420</v>
+      </c>
+      <c r="G25" t="n">
+        <v>425</v>
+      </c>
+      <c r="H25" t="n">
         <v>330</v>
       </c>
-      <c r="F25" t="n">
-        <v>220</v>
-      </c>
-      <c r="G25" t="n">
-        <v>410</v>
-      </c>
-      <c r="H25" t="n">
-        <v>200</v>
-      </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="J25" t="n">
-        <v>2100</v>
+        <v>2105</v>
       </c>
       <c r="K25" t="n">
-        <v>19.35</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Ana Lúcia Teles Rabello</t>
+          <t>Pedro Augusto Alves</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>610</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="D26" t="n">
-        <v>610</v>
+        <v>250</v>
       </c>
       <c r="E26" t="n">
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="F26" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="G26" t="n">
-        <v>180</v>
+        <v>460</v>
       </c>
       <c r="H26" t="n">
-        <v>20</v>
+        <v>380</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="J26" t="n">
-        <v>2090</v>
+        <v>2105</v>
       </c>
       <c r="K26" t="n">
-        <v>58.82</v>
+        <v>65.62</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Taís Nóbrega de Sousa</t>
+          <t>Marina de Moraes Mourão</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>160</v>
+        <v>460</v>
       </c>
       <c r="C27" t="n">
-        <v>260</v>
+        <v>90</v>
       </c>
       <c r="D27" t="n">
-        <v>310</v>
+        <v>390</v>
       </c>
       <c r="E27" t="n">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F27" t="n">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="G27" t="n">
-        <v>350</v>
+        <v>410</v>
       </c>
       <c r="H27" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I27" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>2090</v>
+        <v>2100</v>
       </c>
       <c r="K27" t="n">
-        <v>65.38</v>
+        <v>19.35</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Edward José de Oliveira</t>
+          <t>Ana Lúcia Teles Rabello</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>110</v>
+        <v>610</v>
       </c>
       <c r="C28" t="n">
+        <v>210</v>
+      </c>
+      <c r="D28" t="n">
+        <v>610</v>
+      </c>
+      <c r="E28" t="n">
+        <v>360</v>
+      </c>
+      <c r="F28" t="n">
         <v>100</v>
       </c>
-      <c r="D28" t="n">
-        <v>380</v>
-      </c>
-      <c r="E28" t="n">
-        <v>395</v>
-      </c>
-      <c r="F28" t="n">
-        <v>230</v>
-      </c>
       <c r="G28" t="n">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="H28" t="n">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1955</v>
+        <v>2090</v>
       </c>
       <c r="K28" t="n">
-        <v>27.27</v>
+        <v>58.82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Luzia Helena Carvalho</t>
+          <t>Edward José de Oliveira</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>250</v>
+        <v>110</v>
       </c>
       <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="n">
+        <v>380</v>
+      </c>
+      <c r="E29" t="n">
+        <v>395</v>
+      </c>
+      <c r="F29" t="n">
+        <v>230</v>
+      </c>
+      <c r="G29" t="n">
         <v>350</v>
       </c>
-      <c r="D29" t="n">
-        <v>170</v>
-      </c>
-      <c r="E29" t="n">
-        <v>360</v>
-      </c>
-      <c r="F29" t="n">
-        <v>410</v>
-      </c>
-      <c r="G29" t="n">
-        <v>260</v>
-      </c>
       <c r="H29" t="n">
-        <v>80</v>
+        <v>390</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1880</v>
+        <v>1955</v>
       </c>
       <c r="K29" t="n">
-        <v>72.73</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Roney Santos Coimbra</t>
+          <t>Luzia Helena Carvalho</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>520</v>
+        <v>250</v>
       </c>
       <c r="C30" t="n">
+        <v>350</v>
+      </c>
+      <c r="D30" t="n">
+        <v>170</v>
+      </c>
+      <c r="E30" t="n">
+        <v>360</v>
+      </c>
+      <c r="F30" t="n">
         <v>410</v>
       </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>170</v>
-      </c>
-      <c r="F30" t="n">
-        <v>160</v>
-      </c>
       <c r="G30" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="H30" t="n">
-        <v>420</v>
+        <v>80</v>
       </c>
       <c r="I30" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>1850</v>
+        <v>1880</v>
       </c>
       <c r="K30" t="n">
-        <v>12.5</v>
+        <v>72.73</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Paulo Marcos Zech Coelho</t>
+          <t>Roney Santos Coimbra</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>375</v>
+        <v>520</v>
       </c>
       <c r="C31" t="n">
-        <v>230</v>
+        <v>410</v>
       </c>
       <c r="D31" t="n">
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="F31" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="G31" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H31" t="n">
-        <v>190</v>
+        <v>420</v>
       </c>
       <c r="I31" t="n">
         <v>80</v>
       </c>
       <c r="J31" t="n">
-        <v>1730</v>
+        <v>1850</v>
       </c>
       <c r="K31" t="n">
-        <v>24.24</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Gustavo Fontes Paz</t>
+          <t>Paulo Marcos Zech Coelho</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>550</v>
+        <v>375</v>
       </c>
       <c r="C32" t="n">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="D32" t="n">
-        <v>170</v>
+        <v>435</v>
       </c>
       <c r="E32" t="n">
         <v>260</v>
       </c>
       <c r="F32" t="n">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="G32" t="n">
-        <v>320</v>
+        <v>20</v>
       </c>
       <c r="H32" t="n">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J32" t="n">
-        <v>1710</v>
+        <v>1730</v>
       </c>
       <c r="K32" t="n">
-        <v>26.09</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Roberta Lima Caldeira</t>
+          <t>Gustavo Fontes Paz</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>310</v>
+        <v>550</v>
       </c>
       <c r="C33" t="n">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="D33" t="n">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E33" t="n">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="F33" t="n">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="G33" t="n">
-        <v>220</v>
+        <v>320</v>
       </c>
       <c r="H33" t="n">
-        <v>355</v>
+        <v>60</v>
       </c>
       <c r="I33" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>1685</v>
+        <v>1710</v>
       </c>
       <c r="K33" t="n">
-        <v>16.67</v>
+        <v>26.09</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Marcelo Gustavo Lorenzo</t>
+          <t>Roberta Lima Caldeira</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>180</v>
+        <v>310</v>
       </c>
       <c r="C34" t="n">
+        <v>110</v>
+      </c>
+      <c r="D34" t="n">
         <v>80</v>
       </c>
-      <c r="D34" t="n">
-        <v>170</v>
-      </c>
       <c r="E34" t="n">
-        <v>510</v>
+        <v>280</v>
       </c>
       <c r="F34" t="n">
-        <v>440</v>
+        <v>250</v>
       </c>
       <c r="G34" t="n">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="H34" t="n">
+        <v>355</v>
+      </c>
+      <c r="I34" t="n">
         <v>80</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
       <c r="J34" t="n">
-        <v>1630</v>
+        <v>1685</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Jeronimo Conceição Ruiz</t>
+          <t>Marcelo Gustavo Lorenzo</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>450</v>
+        <v>180</v>
       </c>
       <c r="C35" t="n">
-        <v>220</v>
+        <v>80</v>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="E35" t="n">
-        <v>410</v>
+        <v>510</v>
       </c>
       <c r="F35" t="n">
-        <v>330</v>
+        <v>440</v>
       </c>
       <c r="G35" t="n">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="H35" t="n">
         <v>80</v>
@@ -1745,457 +1745,457 @@
         <v>1630</v>
       </c>
       <c r="K35" t="n">
-        <v>23.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Caroline Furtado Junqueira</t>
+          <t>Jeronimo Conceição Ruiz</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>170</v>
+        <v>450</v>
       </c>
       <c r="C36" t="n">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E36" t="n">
-        <v>360</v>
+        <v>410</v>
       </c>
       <c r="F36" t="n">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="G36" t="n">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="H36" t="n">
-        <v>450</v>
+        <v>80</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1590</v>
+        <v>1630</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Carlos Eduardo Calzavara Silva</t>
+          <t>Caroline Furtado Junqueira</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="C37" t="n">
-        <v>290</v>
+        <v>170</v>
       </c>
       <c r="D37" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="F37" t="n">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="G37" t="n">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="H37" t="n">
-        <v>330</v>
+        <v>450</v>
       </c>
       <c r="I37" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1560</v>
+        <v>1590</v>
       </c>
       <c r="K37" t="n">
-        <v>45.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Cristina Toscano Fonseca</t>
+          <t>Carlos Eduardo Calzavara Silva</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="C38" t="n">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="D38" t="n">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E38" t="n">
-        <v>80</v>
+        <v>330</v>
       </c>
       <c r="F38" t="n">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="G38" t="n">
-        <v>240</v>
+        <v>350</v>
       </c>
       <c r="H38" t="n">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J38" t="n">
-        <v>1450</v>
+        <v>1560</v>
       </c>
       <c r="K38" t="n">
-        <v>30</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Paloma Helena Fernandes Shimabukuro</t>
+          <t>Cristina Toscano Fonseca</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C39" t="n">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E39" t="n">
-        <v>290</v>
+        <v>80</v>
       </c>
       <c r="F39" t="n">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="G39" t="n">
-        <v>310</v>
+        <v>240</v>
       </c>
       <c r="H39" t="n">
-        <v>310</v>
+        <v>350</v>
       </c>
       <c r="I39" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>1415</v>
+        <v>1450</v>
       </c>
       <c r="K39" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Flora Satiko Kano</t>
+          <t>Paloma Helena Fernandes Shimabukuro</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="C40" t="n">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>290</v>
+      </c>
+      <c r="F40" t="n">
         <v>170</v>
       </c>
-      <c r="E40" t="n">
-        <v>260</v>
-      </c>
-      <c r="F40" t="n">
-        <v>250</v>
-      </c>
       <c r="G40" t="n">
-        <v>180</v>
+        <v>310</v>
       </c>
       <c r="H40" t="n">
-        <v>80</v>
+        <v>310</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J40" t="n">
-        <v>1390</v>
+        <v>1415</v>
       </c>
       <c r="K40" t="n">
-        <v>87.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Lileia Gonçalves Diotaiuti</t>
+          <t>Rita de Cássia Moreira de Souza</t>
         </is>
       </c>
       <c r="B41" t="n">
+        <v>270</v>
+      </c>
+      <c r="C41" t="n">
+        <v>95</v>
+      </c>
+      <c r="D41" t="n">
+        <v>280</v>
+      </c>
+      <c r="E41" t="n">
+        <v>110</v>
+      </c>
+      <c r="F41" t="n">
         <v>400</v>
       </c>
-      <c r="C41" t="n">
-        <v>180</v>
-      </c>
-      <c r="D41" t="n">
-        <v>20</v>
-      </c>
-      <c r="E41" t="n">
-        <v>205</v>
-      </c>
-      <c r="F41" t="n">
-        <v>200</v>
-      </c>
       <c r="G41" t="n">
-        <v>240</v>
+        <v>140</v>
       </c>
       <c r="H41" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>1305</v>
+        <v>1405</v>
       </c>
       <c r="K41" t="n">
-        <v>20</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Rafaella Fortini Grenfell e Queiroz</t>
+          <t>Flora Satiko Kano</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="C42" t="n">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="D42" t="n">
-        <v>235</v>
+        <v>170</v>
       </c>
       <c r="E42" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="F42" t="n">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="G42" t="n">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="H42" t="n">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="I42" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>1195</v>
+        <v>1390</v>
       </c>
       <c r="K42" t="n">
-        <v>60.87</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Tânia Maria de Almeida Alves</t>
+          <t>Lileia Gonçalves Diotaiuti</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="C43" t="n">
-        <v>320</v>
+        <v>180</v>
       </c>
       <c r="D43" t="n">
-        <v>210</v>
+        <v>20</v>
       </c>
       <c r="E43" t="n">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="F43" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="G43" t="n">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="H43" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>1185</v>
+        <v>1305</v>
       </c>
       <c r="K43" t="n">
-        <v>31.82</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Érica Alessandra Rocha Alves</t>
+          <t>Rafaella Fortini Grenfell e Queiroz</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="E44" t="n">
-        <v>230</v>
+        <v>90</v>
       </c>
       <c r="F44" t="n">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="G44" t="n">
-        <v>60</v>
+        <v>260</v>
       </c>
       <c r="H44" t="n">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J44" t="n">
-        <v>965</v>
+        <v>1195</v>
       </c>
       <c r="K44" t="n">
-        <v>26.67</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Edelberto Santos Dias</t>
+          <t>Tânia Maria de Almeida Alves</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C45" t="n">
-        <v>170</v>
+        <v>320</v>
       </c>
       <c r="D45" t="n">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E45" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G45" t="n">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="H45" t="n">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>900</v>
+        <v>1185</v>
       </c>
       <c r="K45" t="n">
-        <v>29.41</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Daniel Moreira de Avelar</t>
+          <t>Rosiane Aparecida da Silva Pereira</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D46" t="n">
         <v>190</v>
       </c>
       <c r="E46" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H46" t="n">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="J46" t="n">
-        <v>895</v>
+        <v>980</v>
       </c>
       <c r="K46" t="n">
-        <v>52.94</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Alexandre de Magalhaes Vieira Machado</t>
+          <t>Érica Alessandra Rocha Alves</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>380</v>
+        <v>140</v>
       </c>
       <c r="C47" t="n">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="D47" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="F47" t="n">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>875</v>
+        <v>965</v>
       </c>
       <c r="K47" t="n">
-        <v>25</v>
+        <v>26.67</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Erika Michalsky Monteiro</t>
+          <t>Edelberto Santos Dias</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2205,7 +2205,7 @@
         <v>170</v>
       </c>
       <c r="D48" t="n">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="E48" t="n">
         <v>130</v>
@@ -2217,200 +2217,311 @@
         <v>80</v>
       </c>
       <c r="H48" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="K48" t="n">
-        <v>42.86</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Carina Margonari de Souza</t>
+          <t>Daniel Moreira de Avelar</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C49" t="n">
+        <v>75</v>
+      </c>
+      <c r="D49" t="n">
+        <v>190</v>
+      </c>
+      <c r="E49" t="n">
         <v>100</v>
       </c>
-      <c r="D49" t="n">
-        <v>60</v>
-      </c>
-      <c r="E49" t="n">
-        <v>80</v>
-      </c>
       <c r="F49" t="n">
-        <v>310</v>
+        <v>170</v>
       </c>
       <c r="G49" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="H49" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>790</v>
+        <v>895</v>
       </c>
       <c r="K49" t="n">
-        <v>25</v>
+        <v>52.94</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Álvaro Gil Araújo Ferreira</t>
+          <t>Alexandre de Magalhaes Vieira Machado</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="C50" t="n">
+        <v>85</v>
+      </c>
+      <c r="D50" t="n">
+        <v>150</v>
+      </c>
+      <c r="E50" t="n">
         <v>90</v>
       </c>
-      <c r="D50" t="n">
-        <v>40</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>170</v>
       </c>
-      <c r="F50" t="n">
-        <v>250</v>
-      </c>
       <c r="G50" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>790</v>
+        <v>875</v>
       </c>
       <c r="K50" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Jaquelline Germano de Oliveira</t>
+          <t>Erika Michalsky Monteiro</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C51" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D51" t="n">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="E51" t="n">
-        <v>290</v>
+        <v>130</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I51" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>730</v>
+        <v>800</v>
       </c>
       <c r="K51" t="n">
-        <v>28.57</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Soraya Torres Gaze Jangola</t>
+          <t>Carina Margonari de Souza</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C52" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E52" t="n">
         <v>80</v>
       </c>
       <c r="F52" t="n">
-        <v>175</v>
+        <v>310</v>
       </c>
       <c r="G52" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H52" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>540</v>
+        <v>790</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
+          <t>Álvaro Gil Araújo Ferreira</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>90</v>
+      </c>
+      <c r="D53" t="n">
+        <v>40</v>
+      </c>
+      <c r="E53" t="n">
+        <v>170</v>
+      </c>
+      <c r="F53" t="n">
+        <v>250</v>
+      </c>
+      <c r="G53" t="n">
+        <v>60</v>
+      </c>
+      <c r="H53" t="n">
+        <v>180</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>790</v>
+      </c>
+      <c r="K53" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Jaquelline Germano de Oliveira</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>160</v>
+      </c>
+      <c r="D54" t="n">
+        <v>60</v>
+      </c>
+      <c r="E54" t="n">
+        <v>290</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>140</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>80</v>
+      </c>
+      <c r="J54" t="n">
+        <v>730</v>
+      </c>
+      <c r="K54" t="n">
+        <v>28.57</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>Soraya Torres Gaze Jangola</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>95</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>80</v>
+      </c>
+      <c r="F55" t="n">
+        <v>175</v>
+      </c>
+      <c r="G55" t="n">
+        <v>100</v>
+      </c>
+      <c r="H55" t="n">
+        <v>180</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>630</v>
+      </c>
+      <c r="K55" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
           <t>Marco Antônio da Silva Campos</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="B56" t="n">
         <v>60</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C56" t="n">
         <v>95</v>
       </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
         <v>100</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F56" t="n">
         <v>140</v>
       </c>
-      <c r="G53" t="n">
+      <c r="G56" t="n">
         <v>20</v>
       </c>
-      <c r="H53" t="n">
+      <c r="H56" t="n">
         <v>80</v>
       </c>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="n">
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
         <v>495</v>
       </c>
-      <c r="K53" t="n">
+      <c r="K56" t="n">
         <v>23.08</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado imagens e nomes dos aquivos JSON
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -523,8 +523,10 @@
       <c r="J2" t="n">
         <v>5330</v>
       </c>
-      <c r="K2" t="n">
-        <v>14.89</v>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Alice Paula Di Sabatino Guimarães</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -560,8 +562,10 @@
       <c r="J3" t="n">
         <v>2750</v>
       </c>
-      <c r="K3" t="n">
-        <v>14.29</v>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Ana Cláudia de Araújo Teixeira</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -597,8 +601,10 @@
       <c r="J4" t="n">
         <v>2600</v>
       </c>
-      <c r="K4" t="n">
-        <v>5.26</v>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Ana Camila Oliveira Alves</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -634,8 +640,10 @@
       <c r="J5" t="n">
         <v>2595</v>
       </c>
-      <c r="K5" t="n">
-        <v>14.58</v>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Adriana Costa Bacelo</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -671,8 +679,10 @@
       <c r="J6" t="n">
         <v>2120</v>
       </c>
-      <c r="K6" t="n">
-        <v>10</v>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Anna Carolina Machado Marinho</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -708,8 +718,10 @@
       <c r="J7" t="n">
         <v>1775</v>
       </c>
-      <c r="K7" t="n">
-        <v>15.15</v>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Antonio Marcos Aires Barbosa</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -745,8 +757,10 @@
       <c r="J8" t="n">
         <v>1640</v>
       </c>
-      <c r="K8" t="n">
-        <v>5.88</v>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Anya Pimentel Gomes Fernandes Vieira Meyer</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -782,8 +796,10 @@
       <c r="J9" t="n">
         <v>1490</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Carla Freire Celedonio Fernandes</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -819,8 +835,10 @@
       <c r="J10" t="n">
         <v>1465</v>
       </c>
-      <c r="K10" t="n">
-        <v>48</v>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Claudia Stutz Zubieta</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -856,8 +874,10 @@
       <c r="J11" t="n">
         <v>1415</v>
       </c>
-      <c r="K11" t="n">
-        <v>0</v>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Clarissa Romero Teixeira</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -893,8 +913,10 @@
       <c r="J12" t="n">
         <v>1325</v>
       </c>
-      <c r="K12" t="n">
-        <v>3.7</v>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Dayane Alves Costa</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -930,8 +952,10 @@
       <c r="J13" t="n">
         <v>1190</v>
       </c>
-      <c r="K13" t="n">
-        <v>8.699999999999999</v>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Donat Alexander de Chapeaurouge</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -967,8 +991,10 @@
       <c r="J14" t="n">
         <v>1155</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Eduardo Ruback dos Santos</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1004,8 +1030,10 @@
       <c r="J15" t="n">
         <v>1135</v>
       </c>
-      <c r="K15" t="n">
-        <v>8.699999999999999</v>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Fabio Miyajima</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1041,8 +1069,10 @@
       <c r="J16" t="n">
         <v>1000</v>
       </c>
-      <c r="K16" t="n">
-        <v>20</v>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Fernando Braga Stehling Dias</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1078,8 +1108,10 @@
       <c r="J17" t="n">
         <v>960</v>
       </c>
-      <c r="K17" t="n">
-        <v>9.09</v>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Fernando Ferreira Carneiro</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1115,8 +1147,10 @@
       <c r="J18" t="n">
         <v>920</v>
       </c>
-      <c r="K18" t="n">
-        <v>14.29</v>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Galba Freire Moita</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1152,8 +1186,10 @@
       <c r="J19" t="n">
         <v>740</v>
       </c>
-      <c r="K19" t="n">
-        <v>22.22</v>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1189,8 +1225,10 @@
       <c r="J20" t="n">
         <v>680</v>
       </c>
-      <c r="K20" t="n">
-        <v>5.26</v>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Gilvan Pessoa Furtado</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1226,8 +1264,10 @@
       <c r="J21" t="n">
         <v>675</v>
       </c>
-      <c r="K21" t="n">
-        <v>11.11</v>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Ivana Cristina de Holanda Cunha Barreto</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1263,8 +1303,10 @@
       <c r="J22" t="n">
         <v>640</v>
       </c>
-      <c r="K22" t="n">
-        <v>14.29</v>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Jaime Ribeiro Filho</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1300,8 +1342,10 @@
       <c r="J23" t="n">
         <v>600</v>
       </c>
-      <c r="K23" t="n">
-        <v>9.09</v>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>João Hermínio Martins da Silva</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1337,8 +1381,10 @@
       <c r="J24" t="n">
         <v>360</v>
       </c>
-      <c r="K24" t="n">
-        <v>25</v>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>José Luís Passos Cordeiro</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1374,8 +1420,10 @@
       <c r="J25" t="n">
         <v>300</v>
       </c>
-      <c r="K25" t="n">
-        <v>20</v>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Luiz Odorico Monteiro de Andrade</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1411,8 +1459,10 @@
       <c r="J26" t="n">
         <v>285</v>
       </c>
-      <c r="K26" t="n">
-        <v>30</v>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Marcela Helena Gambim Fonseca</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1448,8 +1498,10 @@
       <c r="J27" t="n">
         <v>270</v>
       </c>
-      <c r="K27" t="n">
-        <v>20</v>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Marcos Roberto Lourenzoni</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1485,8 +1537,10 @@
       <c r="J28" t="n">
         <v>260</v>
       </c>
-      <c r="K28" t="n">
-        <v>0</v>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Márcio Flávio Moura de Araújo</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1522,8 +1576,10 @@
       <c r="J29" t="n">
         <v>260</v>
       </c>
-      <c r="K29" t="n">
-        <v>0</v>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Margareth Borges Coutinho Gallo</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1559,8 +1615,10 @@
       <c r="J30" t="n">
         <v>185</v>
       </c>
-      <c r="K30" t="n">
-        <v>10</v>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Marlos de Medeiros Chaves</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1596,8 +1654,10 @@
       <c r="J31" t="n">
         <v>170</v>
       </c>
-      <c r="K31" t="n">
-        <v>50</v>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Maximiliano Ponte</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1633,8 +1693,10 @@
       <c r="J32" t="n">
         <v>150</v>
       </c>
-      <c r="K32" t="n">
-        <v>100</v>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Raphael Trevizani</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1670,8 +1732,10 @@
       <c r="J33" t="n">
         <v>120</v>
       </c>
-      <c r="K33" t="n">
-        <v>50</v>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Regis Bernardo Brandim Gomes</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1707,8 +1771,10 @@
       <c r="J34" t="n">
         <v>110</v>
       </c>
-      <c r="K34" t="n">
-        <v>50</v>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Roberto Nicolete</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -1744,8 +1810,10 @@
       <c r="J35" t="n">
         <v>100</v>
       </c>
-      <c r="K35" t="n">
-        <v>0</v>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Roberto Wagner Júnior Freire de Freitas</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1781,8 +1849,10 @@
       <c r="J36" t="n">
         <v>100</v>
       </c>
-      <c r="K36" t="n">
-        <v>25</v>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Sharmênia de Araújo Soares Nuto</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1818,8 +1888,10 @@
       <c r="J37" t="n">
         <v>95</v>
       </c>
-      <c r="K37" t="n">
-        <v>100</v>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Vanira Matos Pessoa</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1855,8 +1927,10 @@
       <c r="J38" t="n">
         <v>90</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Venúcia Bruna Magalhães Pereira</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1892,8 +1966,10 @@
       <c r="J39" t="n">
         <v>80</v>
       </c>
-      <c r="K39" t="n">
-        <v>33.33</v>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Fernanda Savicki de Almeida</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1929,8 +2005,10 @@
       <c r="J40" t="n">
         <v>5</v>
       </c>
-      <c r="K40" t="n">
-        <v>0</v>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Caroline Pereira Bittencourt Passaes</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização dados docentes e discentes Fiocruz Ceará
</commit_message>
<xml_diff>
--- a/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/ppgcs_prodpubl_2017_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,7 +720,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Antonio Marcos Aires Barbosa</t>
+          <t>Anya Pimentel Gomes Fernandes Vieira Meyer</t>
         </is>
       </c>
     </row>
@@ -759,85 +759,85 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Anya Pimentel Gomes Fernandes Vieira Meyer</t>
+          <t>Carla Freire Celedonio Fernandes</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Caroline Pereira Bittencourt Passaes</t>
+          <t>Carla Freire Celedonio Fernandes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>90</v>
+        <v>410</v>
       </c>
       <c r="C9" t="n">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="D9" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E9" t="n">
-        <v>360</v>
+        <v>220</v>
       </c>
       <c r="F9" t="n">
-        <v>490</v>
+        <v>320</v>
       </c>
       <c r="G9" t="n">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="H9" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="I9" t="n">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="J9" t="n">
-        <v>1490</v>
+        <v>1525</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Carla Freire Celedonio Fernandes</t>
+          <t>Claudia Stutz Zubieta</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Carla Freire Celedonio Fernandes</t>
+          <t>Caroline Pereira Bittencourt Passaes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>410</v>
+        <v>90</v>
       </c>
       <c r="C10" t="n">
+        <v>90</v>
+      </c>
+      <c r="D10" t="n">
+        <v>110</v>
+      </c>
+      <c r="E10" t="n">
+        <v>360</v>
+      </c>
+      <c r="F10" t="n">
+        <v>490</v>
+      </c>
+      <c r="G10" t="n">
         <v>170</v>
       </c>
-      <c r="D10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E10" t="n">
-        <v>220</v>
-      </c>
-      <c r="F10" t="n">
-        <v>320</v>
-      </c>
-      <c r="G10" t="n">
-        <v>60</v>
-      </c>
       <c r="H10" t="n">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="I10" t="n">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="J10" t="n">
-        <v>1465</v>
+        <v>1490</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Claudia Stutz Zubieta</t>
+          <t>Clarissa Romero Teixeira</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Clarissa Romero Teixeira</t>
+          <t>Dayane Alves Costa</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Dayane Alves Costa</t>
+          <t>Donat Alexander de Chapeaurouge</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Donat Alexander de Chapeaurouge</t>
+          <t>Eduardo Ruback dos Santos</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Eduardo Ruback dos Santos</t>
+          <t>Fabio Miyajima</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Fabio Miyajima</t>
+          <t>Fernando Braga Stehling Dias</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fernando Braga Stehling Dias</t>
+          <t>Fernando Ferreira Carneiro</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Fernando Ferreira Carneiro</t>
+          <t>Galba Freire Moita</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Galba Freire Moita</t>
+          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
+          <t>Gilvan Pessoa Furtado</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Gilvan Pessoa Furtado</t>
+          <t>Ivana Cristina de Holanda Cunha Barreto</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Ivana Cristina de Holanda Cunha Barreto</t>
+          <t>Jaime Ribeiro Filho</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Jaime Ribeiro Filho</t>
+          <t>João Hermínio Martins da Silva</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>João Hermínio Martins da Silva</t>
+          <t>José Luís Passos Cordeiro</t>
         </is>
       </c>
     </row>
@@ -1383,202 +1383,202 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>José Luís Passos Cordeiro</t>
+          <t>Luiz Odorico Monteiro de Andrade</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Marlos de Medeiros Chaves</t>
+          <t>Anna Carolina Machado Marinho</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="G25" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="J25" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Luiz Odorico Monteiro de Andrade</t>
+          <t>Marcela Helena Gambim Fonseca</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Adriana Costa Bacelo</t>
+          <t>Marlos de Medeiros Chaves</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D26" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G26" t="n">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Marcela Helena Gambim Fonseca</t>
+          <t>Marcos Roberto Lourenzoni</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Anna Carolina Machado Marinho</t>
+          <t>Adriana Costa Bacelo</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C27" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H27" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="J27" t="n">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Marcos Roberto Lourenzoni</t>
+          <t>Márcio Flávio Moura de Araújo</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Claudia Stutz Zubieta</t>
+          <t>Venúcia Bruna Magalhães Pereira</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G28" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
         <v>260</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Márcio Flávio Moura de Araújo</t>
+          <t>Margareth Borges Coutinho Gallo</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Venúcia Bruna Magalhães Pereira</t>
+          <t>Claudia Stutz Zubieta</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J29" t="n">
         <v>260</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Margareth Borges Coutinho Gallo</t>
+          <t>Marlos de Medeiros Chaves</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Marlos de Medeiros Chaves</t>
+          <t>Maximiliano Ponte</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Maximiliano Ponte</t>
+          <t>Raphael Trevizani</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Raphael Trevizani</t>
+          <t>Regis Bernardo Brandim Gomes</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Regis Bernardo Brandim Gomes</t>
+          <t>Roberto Nicolete</t>
         </is>
       </c>
     </row>
@@ -1773,18 +1773,18 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Roberto Nicolete</t>
+          <t>Roberto Wagner Júnior Freire de Freitas</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
+          <t>Margareth Borges Coutinho Gallo</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1796,13 +1796,13 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -1812,18 +1812,18 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Roberto Wagner Júnior Freire de Freitas</t>
+          <t>Sharmênia de Araújo Soares Nuto</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Margareth Borges Coutinho Gallo</t>
+          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1835,13 +1835,13 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1851,21 +1851,21 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sharmênia de Araújo Soares Nuto</t>
+          <t>Vanira Matos Pessoa</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Antonio Marcos Aires Barbosa</t>
+          <t>Raphael Trevizani</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -1880,31 +1880,31 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Vanira Matos Pessoa</t>
+          <t>Venúcia Bruna Magalhães Pereira</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Raphael Trevizani</t>
+          <t>Donat Alexander de Chapeaurouge</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1925,25 +1925,25 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Venúcia Bruna Magalhães Pereira</t>
+          <t>Fernanda Savicki de Almeida</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Donat Alexander de Chapeaurouge</t>
+          <t>Fernanda Savicki de Almeida</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -1958,54 +1958,15 @@
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="K39" t="inlineStr">
-        <is>
-          <t>Fernanda Savicki de Almeida</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Fernanda Savicki de Almeida</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>5</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" t="n">
-        <v>5</v>
-      </c>
-      <c r="K40" t="inlineStr">
         <is>
           <t>Caroline Pereira Bittencourt Passaes</t>
         </is>

</xml_diff>